<commit_message>
Tests: Fix tests after solving fixedExch issue
</commit_message>
<xml_diff>
--- a/matlab_code/tests/analysisFxns/testFiles/toy_model1_random2.xlsx
+++ b/matlab_code/tests/analysisFxns/testFiles/toy_model1_random2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -500,8 +500,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="1" sqref="E2:E7 D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,13 +642,16 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,7 +671,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -676,16 +679,18 @@
         <v>-22.0149320730417</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1.10350536706976</v>
+        <f aca="false">0.1*B2</f>
+        <v>-2.20149320730417</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>-22.0149320730417</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1.10350536706976</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.1*D2</f>
+        <v>-2.20149320730417</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -693,16 +698,18 @@
         <v>0.285369137837419</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
+        <f aca="false">0.1*B3</f>
+        <v>0.0285369137837419</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.285369137837419</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.1*D3</f>
+        <v>0.0285369137837419</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -710,16 +717,18 @@
         <v>0.0578197638950879</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
+        <f aca="false">0.1*B4</f>
+        <v>0.00578197638950879</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.0578197638950879</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.1*D4</f>
+        <v>0.00578197638950879</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -727,16 +736,18 @@
         <v>-0.00439408376660814</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
+        <f aca="false">0.1*B5</f>
+        <v>-0.000439408376660814</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>-0.00439408376660814</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.1*D5</f>
+        <v>-0.000439408376660814</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -744,16 +755,18 @@
         <v>6.84865633256387</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
+        <f aca="false">0.1*B6</f>
+        <v>0.684865633256387</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>6.84865633256387</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">0.1*D6</f>
+        <v>0.684865633256387</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -761,13 +774,15 @@
         <v>-0.00242684925806694</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
+        <f aca="false">0.1*B7</f>
+        <v>-0.000242684925806694</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>-0.00242684925806694</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
+        <f aca="false">0.1*D7</f>
+        <v>-0.000242684925806694</v>
       </c>
     </row>
   </sheetData>
@@ -789,7 +804,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E2:E7 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1012,7 +1027,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E2:E7 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1333,7 +1348,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="E2:E7 L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1646,7 +1661,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E2:E7 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2583,7 +2598,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="E2:E7 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3030,7 +3045,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="E2:E7 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3256,7 +3271,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="E2:E7 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3353,7 +3368,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="E2:E7 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3485,7 +3500,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="E2:E7 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3617,7 +3632,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E2:E7 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3798,7 +3813,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="E2:E7 H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>